<commit_message>
COM6053 Final Dashboard Submission
</commit_message>
<xml_diff>
--- a/formatted data.xlsx
+++ b/formatted data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yokohamacu-my.sharepoint.com/personal/d224052d_yokohama-cu_ac_jp/Documents/Leeds授業/Data Science/Assessment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yokohamacu-my.sharepoint.com/personal/d224052d_yokohama-cu_ac_jp/Documents/Leeds授業/Data Science/Assessment/dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{CBB00460-B82A-44F9-9168-5D568187EE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8AD0BD2-EB9C-456F-B7BF-809D8B14791C}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{CBB00460-B82A-44F9-9168-5D568187EE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D258D4EA-B2EE-4569-86C6-2B6750B8B1E7}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{34E2C528-A7FD-4D52-B55E-E2ED29C7EA3F}"/>
+    <workbookView xWindow="10178" yWindow="0" windowWidth="10425" windowHeight="13043" xr2:uid="{34E2C528-A7FD-4D52-B55E-E2ED29C7EA3F}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="168">
   <si>
     <t>all:Sample Size</t>
     <phoneticPr fontId="1"/>
@@ -438,10 +438,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Pre-travel Expenditure</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Group Package Tour</t>
   </si>
   <si>
@@ -451,9 +447,6 @@
     <t>Round-trip Airfare/Ship Fare</t>
   </si>
   <si>
-    <t>Expenditure in Japan</t>
-  </si>
-  <si>
     <t>Accommodation</t>
   </si>
   <si>
@@ -578,6 +571,12 @@
   </si>
   <si>
     <t>Others</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Item</t>
   </si>
 </sst>
 </file>
@@ -771,7 +770,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -880,15 +879,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -943,6 +933,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1264,15 +1258,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A38B46-FA1B-4E10-AB03-E6132E95C1CB}">
   <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <sheetData>
     <row r="1" spans="1:10" ht="38.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>167</v>
+      </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1299,7 +1297,9 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
@@ -5270,10 +5270,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08308FDA-C518-4C8E-B67A-E77B4BD9F3B4}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
@@ -5301,1060 +5301,1038 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="38.25">
       <c r="A2" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="28"/>
+      <c r="B2" s="37">
+        <v>1203</v>
+      </c>
+      <c r="C2" s="38">
+        <v>6.4</v>
+      </c>
+      <c r="D2" s="39">
+        <v>260078</v>
+      </c>
+      <c r="E2" s="40">
+        <v>7</v>
+      </c>
+      <c r="F2" s="38">
+        <v>1.4</v>
+      </c>
+      <c r="G2" s="39">
+        <v>865070</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="38.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="36" t="s">
         <v>122</v>
       </c>
       <c r="B3" s="40">
-        <v>1203</v>
-      </c>
-      <c r="C3" s="41">
-        <v>6.4</v>
-      </c>
-      <c r="D3" s="42">
-        <v>260078</v>
-      </c>
-      <c r="E3" s="43">
-        <v>7</v>
-      </c>
-      <c r="F3" s="41">
-        <v>1.4</v>
-      </c>
-      <c r="G3" s="42">
-        <v>865070</v>
+        <v>605</v>
+      </c>
+      <c r="C3" s="38">
+        <v>3.1</v>
+      </c>
+      <c r="D3" s="39">
+        <v>241686</v>
+      </c>
+      <c r="E3" s="40">
+        <v>10</v>
+      </c>
+      <c r="F3" s="38">
+        <v>2.4</v>
+      </c>
+      <c r="G3" s="39">
+        <v>728454</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="38.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="43">
-        <v>605</v>
-      </c>
-      <c r="C4" s="41">
-        <v>3.1</v>
-      </c>
-      <c r="D4" s="42">
-        <v>241686</v>
-      </c>
-      <c r="E4" s="43">
-        <v>10</v>
-      </c>
-      <c r="F4" s="41">
-        <v>2.4</v>
-      </c>
-      <c r="G4" s="42">
-        <v>728454</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="38.25">
-      <c r="A5" s="44" t="s">
+      <c r="B4" s="42">
+        <v>24220</v>
+      </c>
+      <c r="C4" s="43">
+        <v>90.5</v>
+      </c>
+      <c r="D4" s="44">
+        <v>138004</v>
+      </c>
+      <c r="E4" s="45">
+        <v>566</v>
+      </c>
+      <c r="F4" s="43">
+        <v>96.2</v>
+      </c>
+      <c r="G4" s="44">
+        <v>290888</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="25.5">
+      <c r="A5" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="45">
-        <v>24220</v>
-      </c>
-      <c r="C5" s="46">
-        <v>90.5</v>
-      </c>
-      <c r="D5" s="47">
-        <v>138004</v>
-      </c>
-      <c r="E5" s="48">
-        <v>566</v>
-      </c>
-      <c r="F5" s="46">
-        <v>96.2</v>
-      </c>
-      <c r="G5" s="47">
-        <v>290888</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="B5" s="37">
+        <v>18617</v>
+      </c>
+      <c r="C5" s="38">
+        <v>77.5</v>
+      </c>
+      <c r="D5" s="39">
+        <v>94894</v>
+      </c>
+      <c r="E5" s="40">
+        <v>452</v>
+      </c>
+      <c r="F5" s="38">
+        <v>83.6</v>
+      </c>
+      <c r="G5" s="39">
+        <v>157274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="25.5">
       <c r="A6" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="28"/>
-    </row>
-    <row r="7" spans="1:7" ht="25.5">
-      <c r="A7" s="39" t="s">
+      <c r="B6" s="37">
+        <v>21444</v>
+      </c>
+      <c r="C6" s="38">
+        <v>86.4</v>
+      </c>
+      <c r="D6" s="39">
+        <v>56531</v>
+      </c>
+      <c r="E6" s="40">
+        <v>525</v>
+      </c>
+      <c r="F6" s="38">
+        <v>92.8</v>
+      </c>
+      <c r="G6" s="39">
+        <v>67027</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="26.25">
+      <c r="A7" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="40">
-        <v>18617</v>
-      </c>
-      <c r="C7" s="41">
-        <v>77.5</v>
-      </c>
-      <c r="D7" s="42">
-        <v>94894</v>
-      </c>
-      <c r="E7" s="43">
-        <v>452</v>
-      </c>
-      <c r="F7" s="41">
-        <v>83.6</v>
-      </c>
-      <c r="G7" s="42">
-        <v>157274</v>
+      <c r="B7" s="37">
+        <v>20325</v>
+      </c>
+      <c r="C7" s="38">
+        <v>82.7</v>
+      </c>
+      <c r="D7" s="39">
+        <v>26178</v>
+      </c>
+      <c r="E7" s="40">
+        <v>518</v>
+      </c>
+      <c r="F7" s="38">
+        <v>91.1</v>
+      </c>
+      <c r="G7" s="39">
+        <v>36779</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="25.5">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="40">
-        <v>21444</v>
-      </c>
-      <c r="C8" s="41">
-        <v>86.4</v>
-      </c>
-      <c r="D8" s="42">
-        <v>56531</v>
-      </c>
-      <c r="E8" s="43">
-        <v>525</v>
-      </c>
-      <c r="F8" s="41">
-        <v>92.8</v>
-      </c>
-      <c r="G8" s="42">
-        <v>67027</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="26.25">
-      <c r="A9" s="49" t="s">
+      <c r="B8" s="37">
+        <v>1401</v>
+      </c>
+      <c r="C8" s="38">
+        <v>3.6</v>
+      </c>
+      <c r="D8" s="39">
+        <v>32648</v>
+      </c>
+      <c r="E8" s="40">
+        <v>42</v>
+      </c>
+      <c r="F8" s="38">
+        <v>6.6</v>
+      </c>
+      <c r="G8" s="39">
+        <v>35783</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="25.5">
+      <c r="A9" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="40">
-        <v>20325</v>
-      </c>
-      <c r="C9" s="41">
-        <v>82.7</v>
-      </c>
-      <c r="D9" s="42">
-        <v>26178</v>
-      </c>
-      <c r="E9" s="43">
-        <v>518</v>
-      </c>
-      <c r="F9" s="41">
-        <v>91.1</v>
-      </c>
-      <c r="G9" s="42">
-        <v>36779</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="25.5">
-      <c r="A10" s="39" t="s">
+      <c r="B9" s="37">
+        <v>1395</v>
+      </c>
+      <c r="C9" s="38">
+        <v>7.3</v>
+      </c>
+      <c r="D9" s="39">
+        <v>28664</v>
+      </c>
+      <c r="E9" s="40">
+        <v>71</v>
+      </c>
+      <c r="F9" s="38">
+        <v>16</v>
+      </c>
+      <c r="G9" s="39">
+        <v>43131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="38.25">
+      <c r="A10" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="B10" s="40">
-        <v>1401</v>
-      </c>
-      <c r="C10" s="41">
+      <c r="B10" s="37">
+        <v>15730</v>
+      </c>
+      <c r="C10" s="38">
+        <v>66</v>
+      </c>
+      <c r="D10" s="39">
+        <v>16271</v>
+      </c>
+      <c r="E10" s="40">
+        <v>405</v>
+      </c>
+      <c r="F10" s="38">
+        <v>73.3</v>
+      </c>
+      <c r="G10" s="39">
+        <v>19047</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="37">
+        <v>3806</v>
+      </c>
+      <c r="C11" s="38">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D11" s="39">
+        <v>5493</v>
+      </c>
+      <c r="E11" s="40">
+        <v>75</v>
+      </c>
+      <c r="F11" s="38">
+        <v>12.6</v>
+      </c>
+      <c r="G11" s="39">
+        <v>3652</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="37">
+        <v>6646</v>
+      </c>
+      <c r="C12" s="38">
+        <v>25.2</v>
+      </c>
+      <c r="D12" s="39">
+        <v>14764</v>
+      </c>
+      <c r="E12" s="40">
+        <v>237</v>
+      </c>
+      <c r="F12" s="38">
+        <v>41.4</v>
+      </c>
+      <c r="G12" s="39">
+        <v>17153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="25.5">
+      <c r="A13" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="37">
+        <v>1132</v>
+      </c>
+      <c r="C13" s="38">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D13" s="39">
+        <v>37484</v>
+      </c>
+      <c r="E13" s="40">
+        <v>15</v>
+      </c>
+      <c r="F13" s="38">
+        <v>2.9</v>
+      </c>
+      <c r="G13" s="39">
+        <v>65942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="38.25">
+      <c r="A14" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="40">
+        <v>128</v>
+      </c>
+      <c r="C14" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="39">
+        <v>7525</v>
+      </c>
+      <c r="E14" s="40">
+        <v>7</v>
+      </c>
+      <c r="F14" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="G14" s="39">
+        <v>9993</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="38.25">
+      <c r="A15" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="37">
+        <v>1523</v>
+      </c>
+      <c r="C15" s="38">
+        <v>3.7</v>
+      </c>
+      <c r="D15" s="39">
+        <v>26055</v>
+      </c>
+      <c r="E15" s="40">
+        <v>27</v>
+      </c>
+      <c r="F15" s="38">
         <v>3.6</v>
       </c>
-      <c r="D10" s="42">
-        <v>32648</v>
-      </c>
-      <c r="E10" s="43">
-        <v>42</v>
-      </c>
-      <c r="F10" s="41">
-        <v>6.6</v>
-      </c>
-      <c r="G10" s="42">
-        <v>35783</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="25.5">
-      <c r="A11" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="40">
-        <v>1395</v>
-      </c>
-      <c r="C11" s="41">
-        <v>7.3</v>
-      </c>
-      <c r="D11" s="42">
-        <v>28664</v>
-      </c>
-      <c r="E11" s="43">
-        <v>71</v>
-      </c>
-      <c r="F11" s="41">
+      <c r="G15" s="39">
+        <v>19450</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="39.4">
+      <c r="A16" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="37">
+        <v>9727</v>
+      </c>
+      <c r="C16" s="38">
+        <v>40.6</v>
+      </c>
+      <c r="D16" s="39">
+        <v>36345</v>
+      </c>
+      <c r="E16" s="40">
+        <v>259</v>
+      </c>
+      <c r="F16" s="38">
+        <v>43.8</v>
+      </c>
+      <c r="G16" s="39">
+        <v>16459</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="25.5">
+      <c r="A17" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="40">
+        <v>548</v>
+      </c>
+      <c r="C17" s="38">
+        <v>3.7</v>
+      </c>
+      <c r="D17" s="39">
+        <v>18093</v>
+      </c>
+      <c r="E17" s="40">
         <v>16</v>
       </c>
-      <c r="G11" s="42">
-        <v>43131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="38.25">
-      <c r="A12" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="40">
-        <v>15730</v>
-      </c>
-      <c r="C12" s="41">
-        <v>66</v>
-      </c>
-      <c r="D12" s="42">
-        <v>16271</v>
-      </c>
-      <c r="E12" s="43">
-        <v>405</v>
-      </c>
-      <c r="F12" s="41">
-        <v>73.3</v>
-      </c>
-      <c r="G12" s="42">
-        <v>19047</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" s="40">
-        <v>3806</v>
-      </c>
-      <c r="C13" s="41">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="D13" s="42">
-        <v>5493</v>
-      </c>
-      <c r="E13" s="43">
+      <c r="F17" s="38">
+        <v>3.4</v>
+      </c>
+      <c r="G17" s="39">
+        <v>7149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="38.25">
+      <c r="A18" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="40">
+        <v>172</v>
+      </c>
+      <c r="C18" s="38">
+        <v>0.6</v>
+      </c>
+      <c r="D18" s="39">
+        <v>36728</v>
+      </c>
+      <c r="E18" s="40">
+        <v>5</v>
+      </c>
+      <c r="F18" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="39">
+        <v>10273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="25.5">
+      <c r="A19" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="37">
+        <v>1923</v>
+      </c>
+      <c r="C19" s="38">
+        <v>11</v>
+      </c>
+      <c r="D19" s="39">
+        <v>13395</v>
+      </c>
+      <c r="E19" s="40">
+        <v>51</v>
+      </c>
+      <c r="F19" s="38">
+        <v>11.1</v>
+      </c>
+      <c r="G19" s="39">
+        <v>9719</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="25.5">
+      <c r="A20" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="40">
+        <v>293</v>
+      </c>
+      <c r="C20" s="38">
+        <v>1.4</v>
+      </c>
+      <c r="D20" s="39">
+        <v>21607</v>
+      </c>
+      <c r="E20" s="40">
+        <v>12</v>
+      </c>
+      <c r="F20" s="38">
+        <v>2.4</v>
+      </c>
+      <c r="G20" s="39">
+        <v>16393</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="25.5">
+      <c r="A21" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21" s="40">
+        <v>208</v>
+      </c>
+      <c r="C21" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="39">
+        <v>23785</v>
+      </c>
+      <c r="E21" s="40">
+        <v>11</v>
+      </c>
+      <c r="F21" s="38">
+        <v>1.4</v>
+      </c>
+      <c r="G21" s="39">
+        <v>7531</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="38.25">
+      <c r="A22" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="37">
+        <v>3949</v>
+      </c>
+      <c r="C22" s="38">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D22" s="39">
+        <v>4806</v>
+      </c>
+      <c r="E22" s="40">
+        <v>162</v>
+      </c>
+      <c r="F22" s="38">
+        <v>30.6</v>
+      </c>
+      <c r="G22" s="39">
+        <v>5351</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" s="40">
+        <v>114</v>
+      </c>
+      <c r="C23" s="38">
+        <v>0.3</v>
+      </c>
+      <c r="D23" s="39">
+        <v>15635</v>
+      </c>
+      <c r="E23" s="40">
+        <v>7</v>
+      </c>
+      <c r="F23" s="38">
+        <v>0.3</v>
+      </c>
+      <c r="G23" s="39">
+        <v>32899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="38.25">
+      <c r="A24" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" s="37">
+        <v>1090</v>
+      </c>
+      <c r="C24" s="38">
+        <v>5.9</v>
+      </c>
+      <c r="D24" s="39">
+        <v>7324</v>
+      </c>
+      <c r="E24" s="40">
+        <v>37</v>
+      </c>
+      <c r="F24" s="38">
+        <v>6.8</v>
+      </c>
+      <c r="G24" s="39">
+        <v>6868</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="37">
+        <v>3333</v>
+      </c>
+      <c r="C25" s="38">
+        <v>7.8</v>
+      </c>
+      <c r="D25" s="39">
+        <v>37610</v>
+      </c>
+      <c r="E25" s="40">
+        <v>54</v>
+      </c>
+      <c r="F25" s="38">
+        <v>5</v>
+      </c>
+      <c r="G25" s="39">
+        <v>34328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="63.75">
+      <c r="A26" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="45">
+        <v>117</v>
+      </c>
+      <c r="C26" s="43">
+        <v>0.6</v>
+      </c>
+      <c r="D26" s="44">
+        <v>19557</v>
+      </c>
+      <c r="E26" s="45">
+        <v>1</v>
+      </c>
+      <c r="F26" s="43">
+        <v>0.2</v>
+      </c>
+      <c r="G26" s="44">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="51">
+      <c r="A27" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="40">
         <v>75</v>
       </c>
-      <c r="F13" s="41">
-        <v>12.6</v>
-      </c>
-      <c r="G13" s="42">
-        <v>3652</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" s="40">
-        <v>6646</v>
-      </c>
-      <c r="C14" s="41">
-        <v>25.2</v>
-      </c>
-      <c r="D14" s="42">
-        <v>14764</v>
-      </c>
-      <c r="E14" s="43">
-        <v>237</v>
-      </c>
-      <c r="F14" s="41">
-        <v>41.4</v>
-      </c>
-      <c r="G14" s="42">
-        <v>17153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="25.5">
-      <c r="A15" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="40">
-        <v>1132</v>
-      </c>
-      <c r="C15" s="41">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D15" s="42">
-        <v>37484</v>
-      </c>
-      <c r="E15" s="43">
+      <c r="C27" s="38">
+        <v>0.3</v>
+      </c>
+      <c r="D27" s="39">
+        <v>17137</v>
+      </c>
+      <c r="E27" s="40">
+        <v>3</v>
+      </c>
+      <c r="F27" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="39">
+        <v>5781</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="38.25">
+      <c r="A28" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="40">
+        <v>848</v>
+      </c>
+      <c r="C28" s="38">
+        <v>2.8</v>
+      </c>
+      <c r="D28" s="39">
+        <v>266576</v>
+      </c>
+      <c r="E28" s="40">
+        <v>11</v>
+      </c>
+      <c r="F28" s="38">
+        <v>1.8</v>
+      </c>
+      <c r="G28" s="39">
+        <v>74497</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="37">
+        <v>22862</v>
+      </c>
+      <c r="C29" s="38">
+        <v>92.9</v>
+      </c>
+      <c r="D29" s="39">
+        <v>66309</v>
+      </c>
+      <c r="E29" s="40">
+        <v>493</v>
+      </c>
+      <c r="F29" s="38">
+        <v>87.6</v>
+      </c>
+      <c r="G29" s="39">
+        <v>58430</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="51">
+      <c r="A30" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="37">
+        <v>14289</v>
+      </c>
+      <c r="C30" s="38">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="D30" s="39">
+        <v>11866</v>
+      </c>
+      <c r="E30" s="40">
+        <v>231</v>
+      </c>
+      <c r="F30" s="38">
+        <v>42.7</v>
+      </c>
+      <c r="G30" s="39">
+        <v>7683</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="25.5">
+      <c r="A31" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="37">
+        <v>5592</v>
+      </c>
+      <c r="C31" s="38">
+        <v>22.6</v>
+      </c>
+      <c r="D31" s="39">
+        <v>14104</v>
+      </c>
+      <c r="E31" s="40">
+        <v>136</v>
+      </c>
+      <c r="F31" s="38">
+        <v>25.8</v>
+      </c>
+      <c r="G31" s="39">
+        <v>13828</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="25.5">
+      <c r="A32" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" s="37">
+        <v>1214</v>
+      </c>
+      <c r="C32" s="38">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D32" s="39">
+        <v>24203</v>
+      </c>
+      <c r="E32" s="40">
+        <v>22</v>
+      </c>
+      <c r="F32" s="38">
+        <v>3</v>
+      </c>
+      <c r="G32" s="39">
+        <v>18076</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="38.25">
+      <c r="A33" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" s="37">
+        <v>9992</v>
+      </c>
+      <c r="C33" s="38">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="D33" s="39">
+        <v>14371</v>
+      </c>
+      <c r="E33" s="40">
+        <v>210</v>
+      </c>
+      <c r="F33" s="38">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="G33" s="39">
+        <v>15140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="38.25">
+      <c r="A34" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" s="37">
+        <v>3834</v>
+      </c>
+      <c r="C34" s="38">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="D34" s="39">
+        <v>26133</v>
+      </c>
+      <c r="E34" s="40">
+        <v>39</v>
+      </c>
+      <c r="F34" s="38">
+        <v>7.1</v>
+      </c>
+      <c r="G34" s="39">
+        <v>13391</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="38.25">
+      <c r="A35" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" s="37">
+        <v>3035</v>
+      </c>
+      <c r="C35" s="38">
+        <v>17.3</v>
+      </c>
+      <c r="D35" s="39">
+        <v>15869</v>
+      </c>
+      <c r="E35" s="40">
         <v>15</v>
       </c>
-      <c r="F15" s="41">
-        <v>2.9</v>
-      </c>
-      <c r="G15" s="42">
-        <v>65942</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="38.25">
-      <c r="A16" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" s="43">
-        <v>128</v>
-      </c>
-      <c r="C16" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="D16" s="42">
-        <v>7525</v>
-      </c>
-      <c r="E16" s="43">
-        <v>7</v>
-      </c>
-      <c r="F16" s="41">
+      <c r="F35" s="38">
+        <v>2.6</v>
+      </c>
+      <c r="G35" s="39">
+        <v>11358</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="38.25">
+      <c r="A36" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" s="37">
+        <v>1636</v>
+      </c>
+      <c r="C36" s="38">
+        <v>8.1</v>
+      </c>
+      <c r="D36" s="39">
+        <v>17289</v>
+      </c>
+      <c r="E36" s="40">
+        <v>14</v>
+      </c>
+      <c r="F36" s="38">
+        <v>2.1</v>
+      </c>
+      <c r="G36" s="39">
+        <v>9280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" s="37">
+        <v>7949</v>
+      </c>
+      <c r="C37" s="38">
+        <v>33.1</v>
+      </c>
+      <c r="D37" s="39">
+        <v>31408</v>
+      </c>
+      <c r="E37" s="40">
+        <v>171</v>
+      </c>
+      <c r="F37" s="38">
+        <v>29</v>
+      </c>
+      <c r="G37" s="39">
+        <v>27329</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="38.25">
+      <c r="A38" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="B38" s="37">
+        <v>3989</v>
+      </c>
+      <c r="C38" s="38">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="D38" s="39">
+        <v>57309</v>
+      </c>
+      <c r="E38" s="40">
+        <v>50</v>
+      </c>
+      <c r="F38" s="38">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G38" s="39">
+        <v>156861</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="25.5">
+      <c r="A39" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="B39" s="37">
+        <v>1462</v>
+      </c>
+      <c r="C39" s="38">
+        <v>5.7</v>
+      </c>
+      <c r="D39" s="39">
+        <v>59877</v>
+      </c>
+      <c r="E39" s="40">
+        <v>37</v>
+      </c>
+      <c r="F39" s="38">
+        <v>7.2</v>
+      </c>
+      <c r="G39" s="39">
+        <v>47640</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="25.5">
+      <c r="A40" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" s="40">
+        <v>568</v>
+      </c>
+      <c r="C40" s="38">
+        <v>2.5</v>
+      </c>
+      <c r="D40" s="39">
+        <v>115392</v>
+      </c>
+      <c r="E40" s="40">
+        <v>6</v>
+      </c>
+      <c r="F40" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="G40" s="39">
+        <v>145415</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="38.25">
+      <c r="A41" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="B41" s="40">
+        <v>407</v>
+      </c>
+      <c r="C41" s="38">
         <v>1.5</v>
       </c>
-      <c r="G16" s="42">
-        <v>9993</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="38.25">
-      <c r="A17" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="B17" s="40">
-        <v>1523</v>
-      </c>
-      <c r="C17" s="41">
-        <v>3.7</v>
-      </c>
-      <c r="D17" s="42">
-        <v>26055</v>
-      </c>
-      <c r="E17" s="43">
-        <v>27</v>
-      </c>
-      <c r="F17" s="41">
-        <v>3.6</v>
-      </c>
-      <c r="G17" s="42">
-        <v>19450</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="39.4">
-      <c r="A18" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="B18" s="40">
-        <v>9727</v>
-      </c>
-      <c r="C18" s="41">
-        <v>40.6</v>
-      </c>
-      <c r="D18" s="42">
-        <v>36345</v>
-      </c>
-      <c r="E18" s="43">
-        <v>259</v>
-      </c>
-      <c r="F18" s="41">
-        <v>43.8</v>
-      </c>
-      <c r="G18" s="42">
-        <v>16459</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="25.5">
-      <c r="A19" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="B19" s="43">
-        <v>548</v>
-      </c>
-      <c r="C19" s="41">
-        <v>3.7</v>
-      </c>
-      <c r="D19" s="42">
-        <v>18093</v>
-      </c>
-      <c r="E19" s="43">
-        <v>16</v>
-      </c>
-      <c r="F19" s="41">
-        <v>3.4</v>
-      </c>
-      <c r="G19" s="42">
-        <v>7149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="38.25">
-      <c r="A20" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="B20" s="43">
-        <v>172</v>
-      </c>
-      <c r="C20" s="41">
-        <v>0.6</v>
-      </c>
-      <c r="D20" s="42">
-        <v>36728</v>
-      </c>
-      <c r="E20" s="43">
-        <v>5</v>
-      </c>
-      <c r="F20" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="G20" s="42">
-        <v>10273</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="25.5">
-      <c r="A21" s="39" t="s">
-        <v>140</v>
-      </c>
-      <c r="B21" s="40">
-        <v>1923</v>
-      </c>
-      <c r="C21" s="41">
-        <v>11</v>
-      </c>
-      <c r="D21" s="42">
-        <v>13395</v>
-      </c>
-      <c r="E21" s="43">
-        <v>51</v>
-      </c>
-      <c r="F21" s="41">
-        <v>11.1</v>
-      </c>
-      <c r="G21" s="42">
-        <v>9719</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="25.5">
-      <c r="A22" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="43">
-        <v>293</v>
-      </c>
-      <c r="C22" s="41">
-        <v>1.4</v>
-      </c>
-      <c r="D22" s="42">
-        <v>21607</v>
-      </c>
-      <c r="E22" s="43">
+      <c r="D41" s="39">
+        <v>162400</v>
+      </c>
+      <c r="E41" s="40">
         <v>12</v>
       </c>
-      <c r="F22" s="41">
-        <v>2.4</v>
-      </c>
-      <c r="G22" s="42">
-        <v>16393</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="25.5">
-      <c r="A23" s="39" t="s">
-        <v>142</v>
-      </c>
-      <c r="B23" s="43">
-        <v>208</v>
-      </c>
-      <c r="C23" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="D23" s="42">
-        <v>23785</v>
-      </c>
-      <c r="E23" s="43">
-        <v>11</v>
-      </c>
-      <c r="F23" s="41">
-        <v>1.4</v>
-      </c>
-      <c r="G23" s="42">
-        <v>7531</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="38.25">
-      <c r="A24" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="B24" s="40">
-        <v>3949</v>
-      </c>
-      <c r="C24" s="41">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="D24" s="42">
-        <v>4806</v>
-      </c>
-      <c r="E24" s="43">
+      <c r="F41" s="38">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G41" s="39">
+        <v>67875</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="38.25">
+      <c r="A42" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="B42" s="37">
+        <v>2097</v>
+      </c>
+      <c r="C42" s="38">
+        <v>6.9</v>
+      </c>
+      <c r="D42" s="39">
+        <v>17890</v>
+      </c>
+      <c r="E42" s="40">
+        <v>104</v>
+      </c>
+      <c r="F42" s="38">
+        <v>20</v>
+      </c>
+      <c r="G42" s="39">
+        <v>13355</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="25.5">
+      <c r="A43" s="47" t="s">
         <v>162</v>
       </c>
-      <c r="F24" s="41">
-        <v>30.6</v>
-      </c>
-      <c r="G24" s="42">
-        <v>5351</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" s="43">
-        <v>114</v>
-      </c>
-      <c r="C25" s="41">
+      <c r="B43" s="37">
+        <v>1244</v>
+      </c>
+      <c r="C43" s="38">
+        <v>4.3</v>
+      </c>
+      <c r="D43" s="39">
+        <v>10534</v>
+      </c>
+      <c r="E43" s="40">
+        <v>46</v>
+      </c>
+      <c r="F43" s="38">
+        <v>8.6</v>
+      </c>
+      <c r="G43" s="39">
+        <v>7843</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="38.25">
+      <c r="A44" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="40">
+        <v>634</v>
+      </c>
+      <c r="C44" s="38">
+        <v>2.7</v>
+      </c>
+      <c r="D44" s="39">
+        <v>22352</v>
+      </c>
+      <c r="E44" s="40">
+        <v>22</v>
+      </c>
+      <c r="F44" s="38">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G44" s="39">
+        <v>25638</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="25.5">
+      <c r="A45" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" s="37">
+        <v>1655</v>
+      </c>
+      <c r="C45" s="38">
+        <v>7.4</v>
+      </c>
+      <c r="D45" s="39">
+        <v>30425</v>
+      </c>
+      <c r="E45" s="40">
+        <v>46</v>
+      </c>
+      <c r="F45" s="38">
+        <v>9.4</v>
+      </c>
+      <c r="G45" s="39">
+        <v>44786</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="B46" s="45">
+        <v>44</v>
+      </c>
+      <c r="C46" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="D46" s="44">
+        <v>99374</v>
+      </c>
+      <c r="E46" s="45">
+        <v>2</v>
+      </c>
+      <c r="F46" s="43">
         <v>0.3</v>
       </c>
-      <c r="D25" s="42">
-        <v>15635</v>
-      </c>
-      <c r="E25" s="43">
-        <v>7</v>
-      </c>
-      <c r="F25" s="41">
-        <v>0.3</v>
-      </c>
-      <c r="G25" s="42">
-        <v>32899</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="38.25">
-      <c r="A26" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="B26" s="40">
-        <v>1090</v>
-      </c>
-      <c r="C26" s="41">
-        <v>5.9</v>
-      </c>
-      <c r="D26" s="42">
-        <v>7324</v>
-      </c>
-      <c r="E26" s="43">
-        <v>37</v>
-      </c>
-      <c r="F26" s="41">
-        <v>6.8</v>
-      </c>
-      <c r="G26" s="42">
-        <v>6868</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="B27" s="40">
-        <v>3333</v>
-      </c>
-      <c r="C27" s="41">
-        <v>7.8</v>
-      </c>
-      <c r="D27" s="42">
-        <v>37610</v>
-      </c>
-      <c r="E27" s="43">
-        <v>54</v>
-      </c>
-      <c r="F27" s="41">
-        <v>5</v>
-      </c>
-      <c r="G27" s="42">
-        <v>34328</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="63.75">
-      <c r="A28" s="44" t="s">
-        <v>147</v>
-      </c>
-      <c r="B28" s="48">
-        <v>117</v>
-      </c>
-      <c r="C28" s="46">
-        <v>0.6</v>
-      </c>
-      <c r="D28" s="47">
-        <v>19557</v>
-      </c>
-      <c r="E28" s="48">
-        <v>1</v>
-      </c>
-      <c r="F28" s="46">
-        <v>0.2</v>
-      </c>
-      <c r="G28" s="47">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="51">
-      <c r="A29" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="B29" s="43">
-        <v>75</v>
-      </c>
-      <c r="C29" s="41">
-        <v>0.3</v>
-      </c>
-      <c r="D29" s="42">
-        <v>17137</v>
-      </c>
-      <c r="E29" s="43">
-        <v>3</v>
-      </c>
-      <c r="F29" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="G29" s="42">
-        <v>5781</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="38.25">
-      <c r="A30" s="50" t="s">
-        <v>149</v>
-      </c>
-      <c r="B30" s="43">
-        <v>848</v>
-      </c>
-      <c r="C30" s="41">
-        <v>2.8</v>
-      </c>
-      <c r="D30" s="42">
-        <v>266576</v>
-      </c>
-      <c r="E30" s="43">
-        <v>11</v>
-      </c>
-      <c r="F30" s="41">
-        <v>1.8</v>
-      </c>
-      <c r="G30" s="42">
-        <v>74497</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="51" t="s">
-        <v>150</v>
-      </c>
-      <c r="B31" s="40">
-        <v>22862</v>
-      </c>
-      <c r="C31" s="41">
-        <v>92.9</v>
-      </c>
-      <c r="D31" s="42">
-        <v>66309</v>
-      </c>
-      <c r="E31" s="43">
-        <v>493</v>
-      </c>
-      <c r="F31" s="41">
-        <v>87.6</v>
-      </c>
-      <c r="G31" s="42">
-        <v>58430</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="51">
-      <c r="A32" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="B32" s="40">
-        <v>14289</v>
-      </c>
-      <c r="C32" s="41">
-        <v>64.400000000000006</v>
-      </c>
-      <c r="D32" s="42">
-        <v>11866</v>
-      </c>
-      <c r="E32" s="43">
-        <v>231</v>
-      </c>
-      <c r="F32" s="41">
-        <v>42.7</v>
-      </c>
-      <c r="G32" s="42">
-        <v>7683</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="25.5">
-      <c r="A33" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="B33" s="40">
-        <v>5592</v>
-      </c>
-      <c r="C33" s="41">
-        <v>22.6</v>
-      </c>
-      <c r="D33" s="42">
-        <v>14104</v>
-      </c>
-      <c r="E33" s="43">
-        <v>136</v>
-      </c>
-      <c r="F33" s="41">
-        <v>25.8</v>
-      </c>
-      <c r="G33" s="42">
-        <v>13828</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="25.5">
-      <c r="A34" s="50" t="s">
-        <v>153</v>
-      </c>
-      <c r="B34" s="40">
-        <v>1214</v>
-      </c>
-      <c r="C34" s="41">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="D34" s="42">
-        <v>24203</v>
-      </c>
-      <c r="E34" s="43">
-        <v>22</v>
-      </c>
-      <c r="F34" s="41">
-        <v>3</v>
-      </c>
-      <c r="G34" s="42">
-        <v>18076</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="38.25">
-      <c r="A35" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B35" s="40">
-        <v>9992</v>
-      </c>
-      <c r="C35" s="41">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="D35" s="42">
-        <v>14371</v>
-      </c>
-      <c r="E35" s="43">
-        <v>210</v>
-      </c>
-      <c r="F35" s="41">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="G35" s="42">
-        <v>15140</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="38.25">
-      <c r="A36" s="50" t="s">
-        <v>155</v>
-      </c>
-      <c r="B36" s="40">
-        <v>3834</v>
-      </c>
-      <c r="C36" s="41">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="D36" s="42">
-        <v>26133</v>
-      </c>
-      <c r="E36" s="43">
-        <v>39</v>
-      </c>
-      <c r="F36" s="41">
-        <v>7.1</v>
-      </c>
-      <c r="G36" s="42">
-        <v>13391</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="38.25">
-      <c r="A37" s="50" t="s">
-        <v>156</v>
-      </c>
-      <c r="B37" s="40">
-        <v>3035</v>
-      </c>
-      <c r="C37" s="41">
-        <v>17.3</v>
-      </c>
-      <c r="D37" s="42">
-        <v>15869</v>
-      </c>
-      <c r="E37" s="43">
-        <v>15</v>
-      </c>
-      <c r="F37" s="41">
-        <v>2.6</v>
-      </c>
-      <c r="G37" s="42">
-        <v>11358</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="38.25">
-      <c r="A38" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="B38" s="40">
-        <v>1636</v>
-      </c>
-      <c r="C38" s="41">
-        <v>8.1</v>
-      </c>
-      <c r="D38" s="42">
-        <v>17289</v>
-      </c>
-      <c r="E38" s="43">
-        <v>14</v>
-      </c>
-      <c r="F38" s="41">
-        <v>2.1</v>
-      </c>
-      <c r="G38" s="42">
-        <v>9280</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="B39" s="40">
-        <v>7949</v>
-      </c>
-      <c r="C39" s="41">
-        <v>33.1</v>
-      </c>
-      <c r="D39" s="42">
-        <v>31408</v>
-      </c>
-      <c r="E39" s="43">
-        <v>171</v>
-      </c>
-      <c r="F39" s="41">
-        <v>29</v>
-      </c>
-      <c r="G39" s="42">
-        <v>27329</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="38.25">
-      <c r="A40" s="50" t="s">
-        <v>159</v>
-      </c>
-      <c r="B40" s="40">
-        <v>3989</v>
-      </c>
-      <c r="C40" s="41">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="D40" s="42">
-        <v>57309</v>
-      </c>
-      <c r="E40" s="43">
-        <v>50</v>
-      </c>
-      <c r="F40" s="41">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="G40" s="42">
-        <v>156861</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="25.5">
-      <c r="A41" s="50" t="s">
-        <v>160</v>
-      </c>
-      <c r="B41" s="40">
-        <v>1462</v>
-      </c>
-      <c r="C41" s="41">
-        <v>5.7</v>
-      </c>
-      <c r="D41" s="42">
-        <v>59877</v>
-      </c>
-      <c r="E41" s="43">
-        <v>37</v>
-      </c>
-      <c r="F41" s="41">
-        <v>7.2</v>
-      </c>
-      <c r="G41" s="42">
-        <v>47640</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="25.5">
-      <c r="A42" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="B42" s="43">
-        <v>568</v>
-      </c>
-      <c r="C42" s="41">
-        <v>2.5</v>
-      </c>
-      <c r="D42" s="42">
-        <v>115392</v>
-      </c>
-      <c r="E42" s="43">
-        <v>6</v>
-      </c>
-      <c r="F42" s="41">
-        <v>0.9</v>
-      </c>
-      <c r="G42" s="42">
-        <v>145415</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="38.25">
-      <c r="A43" s="50" t="s">
-        <v>162</v>
-      </c>
-      <c r="B43" s="43">
-        <v>407</v>
-      </c>
-      <c r="C43" s="41">
-        <v>1.5</v>
-      </c>
-      <c r="D43" s="42">
-        <v>162400</v>
-      </c>
-      <c r="E43" s="43">
-        <v>12</v>
-      </c>
-      <c r="F43" s="41">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G43" s="42">
-        <v>67875</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="38.25">
-      <c r="A44" s="50" t="s">
-        <v>163</v>
-      </c>
-      <c r="B44" s="40">
-        <v>2097</v>
-      </c>
-      <c r="C44" s="41">
-        <v>6.9</v>
-      </c>
-      <c r="D44" s="42">
-        <v>17890</v>
-      </c>
-      <c r="E44" s="43">
-        <v>104</v>
-      </c>
-      <c r="F44" s="41">
-        <v>20</v>
-      </c>
-      <c r="G44" s="42">
-        <v>13355</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="25.5">
-      <c r="A45" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="B45" s="40">
-        <v>1244</v>
-      </c>
-      <c r="C45" s="41">
-        <v>4.3</v>
-      </c>
-      <c r="D45" s="42">
-        <v>10534</v>
-      </c>
-      <c r="E45" s="43">
-        <v>46</v>
-      </c>
-      <c r="F45" s="41">
-        <v>8.6</v>
-      </c>
-      <c r="G45" s="42">
-        <v>7843</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="38.25">
-      <c r="A46" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="B46" s="43">
-        <v>634</v>
-      </c>
-      <c r="C46" s="41">
-        <v>2.7</v>
-      </c>
-      <c r="D46" s="42">
-        <v>22352</v>
-      </c>
-      <c r="E46" s="43">
-        <v>22</v>
-      </c>
-      <c r="F46" s="41">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G46" s="42">
-        <v>25638</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="25.5">
-      <c r="A47" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="B47" s="40">
-        <v>1655</v>
-      </c>
-      <c r="C47" s="41">
-        <v>7.4</v>
-      </c>
-      <c r="D47" s="42">
-        <v>30425</v>
-      </c>
-      <c r="E47" s="43">
-        <v>46</v>
-      </c>
-      <c r="F47" s="41">
-        <v>9.4</v>
-      </c>
-      <c r="G47" s="42">
-        <v>44786</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="B48" s="48">
-        <v>44</v>
-      </c>
-      <c r="C48" s="46">
-        <v>0.1</v>
-      </c>
-      <c r="D48" s="47">
-        <v>99374</v>
-      </c>
-      <c r="E48" s="48">
-        <v>2</v>
-      </c>
-      <c r="F48" s="46">
-        <v>0.3</v>
-      </c>
-      <c r="G48" s="47">
+      <c r="G46" s="44">
         <v>25000</v>
       </c>
     </row>

</xml_diff>